<commit_message>
SM: add iteration2 files
</commit_message>
<xml_diff>
--- a/doc/CS673_SPPP_RiskManagement.xlsx
+++ b/doc/CS673_SPPP_RiskManagement.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="120">
   <si>
     <t>This sheet provides some common risks in student projects. You should check if it applies to your group project. 
 You should also feel free to add other risks. Exemplary analysis is also added.</t>
@@ -83,58 +83,61 @@
     <t>Redefine the project scope if necessary, and assign the tasks to other team members.</t>
   </si>
   <si>
-    <t>No one dropped the class so far</t>
+    <t>No one will drop the class</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>add new team members</t>
+  </si>
+  <si>
+    <t>Due to chances of group 7 disbanding, we might get a new team member</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Share Leadership</t>
+  </si>
+  <si>
+    <t>Will not get any new team members at this time</t>
+  </si>
+  <si>
+    <t>Lack of motivation or responsibility</t>
+  </si>
+  <si>
+    <t>Due to conflicting schedules, there can be an imbalance of work done causing lack of motivation and responsibility</t>
+  </si>
+  <si>
+    <t>Samantha Mathis</t>
+  </si>
+  <si>
+    <t>Team leader will motivate demotivated team members</t>
+  </si>
+  <si>
+    <t>Everyone is motivated and we have neared the end of the project</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>duplicate work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some sections are assigned to multiple people due to a higher number of people than sections, which may cause duplicaiton </t>
+  </si>
+  <si>
+    <t>Ahnaf Tajwar</t>
+  </si>
+  <si>
+    <t>As long as we track our user stories and work. There shouldn't be anyone working on something someone already has. Each week we'll having meetings to communicate what each person is currently working on. So even if it does happen we will find out early</t>
+  </si>
+  <si>
+    <t>Communcating and assigning our names to things</t>
   </si>
   <si>
     <t>Open</t>
-  </si>
-  <si>
-    <t>add new team members</t>
-  </si>
-  <si>
-    <t>Due to chances of group 7 disbanding, we might get a new team member</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Share Leadership</t>
-  </si>
-  <si>
-    <t>Extra Meeting to get memeber up to speed</t>
-  </si>
-  <si>
-    <t>Lack of motivation or responsibility</t>
-  </si>
-  <si>
-    <t>Due to conflicting schedules, there can be an imbalance of work done causing lack of motivation and responsibility</t>
-  </si>
-  <si>
-    <t>Samantha Mathis</t>
-  </si>
-  <si>
-    <t>Team leader will motivate demotivated team members</t>
-  </si>
-  <si>
-    <t>Everyone seems super motivated as of week 1</t>
-  </si>
-  <si>
-    <t>Communication</t>
-  </si>
-  <si>
-    <t>duplicate work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Some sections are assigned to multiple people due to a higher number of people than sections, which may cause duplicaiton </t>
-  </si>
-  <si>
-    <t>Ahnaf Tajwar</t>
-  </si>
-  <si>
-    <t>As long as we track our user stories and work. There shouldn't be anyone working on something someone already has. Each week we'll having meetings to communicate what each person is currently working on. So even if it does happen we will find out early</t>
-  </si>
-  <si>
-    <t>Communcating and assigning our names to things</t>
   </si>
   <si>
     <t>worked on wrong components</t>
@@ -247,7 +250,7 @@
     <t>Utilize online resources such as youtube for a quick refresher on key syntax</t>
   </si>
   <si>
-    <t>Started to watch some quick refreshers</t>
+    <t>Everyone got up to speed with languages used</t>
   </si>
   <si>
     <t>Not familiar with unit testing</t>
@@ -261,7 +264,7 @@
 Implement a few unit tests together</t>
   </si>
   <si>
-    <t>Development has not started yet</t>
+    <t>Everyone has completed some unit testing</t>
   </si>
   <si>
     <t>Other technology incompetence</t>
@@ -275,6 +278,9 @@
 Implement a basic application using React</t>
   </si>
   <si>
+    <t>Everyone was able to learn what they needed with React/JS</t>
+  </si>
+  <si>
     <t>Not familiar with Git</t>
   </si>
   <si>
@@ -285,7 +291,7 @@
 Most of us are familiar enough with Git to help those who are not</t>
   </si>
   <si>
-    <t>Everyone has read up on Git as instructed in Lab 1</t>
+    <t>Everyone has read up on Git as instructed in Lab 1 and is now much more comfortable after repeated use</t>
   </si>
   <si>
     <t>Not familiar with general software development and IDE use</t>
@@ -297,7 +303,7 @@
     <t>Reach out to the team whenever having trouble understanding software development process and IDE use</t>
   </si>
   <si>
-    <t>Basic idea of project goal</t>
+    <t>Everyone got more experience with developing software and how to use their IDE</t>
   </si>
   <si>
     <t>Design and implementation</t>
@@ -353,6 +359,9 @@
   </si>
   <si>
     <t>Devlopment and testing will be done simultanesouly</t>
+  </si>
+  <si>
+    <t>Development has not started yet</t>
   </si>
   <si>
     <t>Improper testing tools</t>
@@ -874,7 +883,7 @@
       <c r="J3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="12" t="s">
         <v>19</v>
       </c>
       <c r="L3" s="12" t="s">
@@ -929,7 +938,7 @@
       <c r="K4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="12" t="s">
         <v>20</v>
       </c>
       <c r="M4" s="13"/>
@@ -981,7 +990,7 @@
       <c r="K5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="12" t="s">
         <v>20</v>
       </c>
       <c r="M5" s="13"/>
@@ -1036,7 +1045,7 @@
         <v>36</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -1057,10 +1066,10 @@
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" s="15">
         <v>3.0</v>
@@ -1076,19 +1085,19 @@
         <v>36</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I7" s="16">
         <v>45217.0</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>36</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
@@ -1108,13 +1117,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D8" s="15">
         <v>3.0</v>
@@ -1130,19 +1139,19 @@
         <v>24</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I8" s="16">
         <v>45195.0</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
@@ -1163,10 +1172,10 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="14"/>
       <c r="B9" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D9" s="15">
         <v>2.0</v>
@@ -1182,19 +1191,19 @@
         <v>32</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I9" s="16">
         <v>45195.0</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
@@ -1215,10 +1224,10 @@
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="14"/>
       <c r="B10" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D10" s="15">
         <v>3.0</v>
@@ -1234,19 +1243,19 @@
         <v>30</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I10" s="16">
         <v>45195.0</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
@@ -1266,13 +1275,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" s="15">
         <v>1.0</v>
@@ -1288,19 +1297,19 @@
         <v>60</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I11" s="16">
         <v>45217.0</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
@@ -1321,10 +1330,10 @@
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="14"/>
       <c r="B12" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D12" s="15">
         <v>2.0</v>
@@ -1340,19 +1349,19 @@
         <v>48</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I12" s="16">
         <v>45217.0</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
@@ -1372,13 +1381,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D13" s="15">
         <v>5.0</v>
@@ -1394,19 +1403,19 @@
         <v>9</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I13" s="16">
         <v>45195.0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="M13" s="19"/>
       <c r="N13" s="13"/>
@@ -1427,10 +1436,10 @@
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D14" s="15">
         <v>5.0</v>
@@ -1452,12 +1461,12 @@
         <v>45188.0</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="L14" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" s="12" t="s">
         <v>20</v>
       </c>
       <c r="M14" s="13"/>
@@ -1479,10 +1488,10 @@
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="14"/>
       <c r="B15" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D15" s="15">
         <v>4.0</v>
@@ -1504,12 +1513,12 @@
         <v>45202.0</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="L15" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L15" s="12" t="s">
         <v>20</v>
       </c>
       <c r="M15" s="13"/>
@@ -1531,10 +1540,10 @@
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="14"/>
       <c r="B16" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D16" s="15">
         <v>5.0</v>
@@ -1550,18 +1559,18 @@
         <v>9</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I16" s="16">
         <v>45195.0</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="L16" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L16" s="12" t="s">
         <v>20</v>
       </c>
       <c r="M16" s="13"/>
@@ -1583,10 +1592,10 @@
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="14"/>
       <c r="B17" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D17" s="15">
         <v>4.0</v>
@@ -1608,12 +1617,12 @@
         <v>45188.0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="L17" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" s="12" t="s">
         <v>20</v>
       </c>
       <c r="M17" s="13"/>
@@ -1635,10 +1644,10 @@
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="14"/>
       <c r="B18" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D18" s="15">
         <v>2.0</v>
@@ -1660,12 +1669,12 @@
         <v>45188.0</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="L18" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="L18" s="12" t="s">
         <v>20</v>
       </c>
       <c r="M18" s="13"/>
@@ -1686,13 +1695,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="14" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D19" s="15">
         <v>3.0</v>
@@ -1708,18 +1717,18 @@
         <v>24</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I19" s="16">
         <v>45195.0</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="L19" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="L19" s="12" t="s">
         <v>20</v>
       </c>
       <c r="M19" s="13"/>
@@ -1741,10 +1750,10 @@
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="14"/>
       <c r="B20" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D20" s="15">
         <v>2.0</v>
@@ -1760,18 +1769,18 @@
         <v>32</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I20" s="16">
         <v>45195.0</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="L20" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="L20" s="12" t="s">
         <v>20</v>
       </c>
       <c r="M20" s="13"/>
@@ -1793,10 +1802,10 @@
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="14"/>
       <c r="B21" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D21" s="15">
         <v>4.0</v>
@@ -1812,19 +1821,19 @@
         <v>16</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I21" s="16">
         <v>45217.0</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>20</v>
+        <v>96</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
@@ -1844,13 +1853,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="14" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D22" s="15">
         <v>2.0</v>
@@ -1865,19 +1874,19 @@
         <v>4.0</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I22" s="16">
         <v>45195.0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="M22" s="19"/>
       <c r="N22" s="13"/>
@@ -1898,10 +1907,10 @@
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="14"/>
       <c r="B23" s="17" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D23" s="15">
         <v>2.0</v>
@@ -1916,18 +1925,18 @@
         <v>3.0</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I23" s="16">
         <v>45195.0</v>
       </c>
       <c r="J23" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="K23" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="K23" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="L23" s="7" t="s">
+      <c r="L23" s="12" t="s">
         <v>20</v>
       </c>
       <c r="M23" s="19"/>
@@ -1948,13 +1957,13 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="14" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D24" s="15">
         <v>2.0</v>
@@ -1969,19 +1978,19 @@
         <v>3.0</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I24" s="16">
         <v>45195.0</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="M24" s="19"/>
       <c r="N24" s="13"/>
@@ -2002,10 +2011,10 @@
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="6"/>
       <c r="B25" s="17" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D25" s="15">
         <v>2.0</v>
@@ -2020,18 +2029,18 @@
         <v>4.0</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I25" s="16">
         <v>45195.0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="L25" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L25" s="12" t="s">
         <v>20</v>
       </c>
       <c r="M25" s="13"/>

</xml_diff>